<commit_message>
modified file to enhance image viewing
</commit_message>
<xml_diff>
--- a/files/attention_visual.xlsx
+++ b/files/attention_visual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\General_Code\newSite\pratik-doshi-99.github.io\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5994C90-4B1E-4656-B902-03FB239EFF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE3B638-3A19-47A1-B98C-20B18356BD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28995" yWindow="-195" windowWidth="29190" windowHeight="15870" xr2:uid="{46AF5287-2058-4E5D-902D-DB2F884B6C9C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{46AF5287-2058-4E5D-902D-DB2F884B6C9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
     <t>A.T @ V</t>
   </si>
   <si>
-    <t>A is transposed because it is generated inverted for visualizing its distribution</t>
+    <t>A is transposed because it is generated invertedly for visualizing its distribution. Transpose is not part of the attention operation</t>
   </si>
 </sst>
 </file>
@@ -220,7 +220,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -229,10 +229,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -241,7 +241,7 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -253,16 +253,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -580,50 +580,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FBF36BD-3F81-4061-AD73-9D0BAE013D4B}">
-  <dimension ref="B12:X18"/>
+  <dimension ref="B11:X18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Z34" sqref="Z34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="3.73046875" customWidth="1"/>
     <col min="2" max="2" width="8.265625" customWidth="1"/>
     <col min="3" max="6" width="7.06640625" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" customWidth="1"/>
-    <col min="24" max="24" width="9.06640625" customWidth="1"/>
+    <col min="7" max="7" width="1.86328125" customWidth="1"/>
+    <col min="9" max="15" width="7.19921875" customWidth="1"/>
+    <col min="16" max="16" width="2.3984375" customWidth="1"/>
+    <col min="17" max="24" width="7.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.45">
-      <c r="B12" s="17" t="s">
+    <row r="11" spans="2:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="2:24" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="H12" s="18" t="s">
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="H12" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="Q12" s="18" t="s">
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="Q12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
     </row>
-    <row r="13" spans="2:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="1"/>
       <c r="C13" s="5" t="s">
         <v>0</v>
@@ -638,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="Q13" s="19"/>
+      <c r="Q13" s="17"/>
       <c r="R13" s="20" t="s">
         <v>15</v>
       </c>
@@ -649,7 +653,7 @@
       <c r="W13" s="20"/>
       <c r="X13" s="20"/>
     </row>
-    <row r="14" spans="2:24" ht="39.85" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:24" ht="47.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
@@ -722,7 +726,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="2:24" ht="39.85" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:24" ht="47.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
@@ -795,7 +799,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="16" spans="2:24" ht="39.85" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:24" ht="47.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="4" t="s">
         <v>6</v>
       </c>
@@ -868,7 +872,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="17" spans="2:24" ht="39.85" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:24" ht="47.35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
@@ -941,7 +945,7 @@
         <v>0.35000000000000003</v>
       </c>
     </row>
-    <row r="18" spans="2:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:24" ht="24.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="2"/>
       <c r="C18" s="10">
         <f>SUM(C14:C17)</f>
@@ -978,6 +982,20 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{AEFF7FE2-5391-47A5-96D5-007B52E58A62}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:G17">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2A26DABB-399A-4CCC-82E9-F0EB5185F719}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1024,20 +1042,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:G17">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2A26DABB-399A-4CCC-82E9-F0EB5185F719}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -1055,6 +1059,17 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>C14:C17</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2A26DABB-399A-4CCC-82E9-F0EB5185F719}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0" direction="rightToLeft">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C14:G17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E4A4F044-C678-4C04-8A2F-146CDEA7F319}">
@@ -1093,17 +1108,6 @@
           </x14:cfRule>
           <xm:sqref>F14:G17</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2A26DABB-399A-4CCC-82E9-F0EB5185F719}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0" direction="rightToLeft">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>C14:G17</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>